<commit_message>
permision denied fixed in grooming algorithm
</commit_message>
<xml_diff>
--- a/esfahan/node_esfahan.xlsx
+++ b/esfahan/node_esfahan.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="62">
   <si>
     <t>ID</t>
   </si>
@@ -162,9 +162,6 @@
   </si>
   <si>
     <t>ERD</t>
-  </si>
-  <si>
-    <t>32.661244, 51.677711</t>
   </si>
   <si>
     <t>EFZ</t>
@@ -1753,10 +1750,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1793,7 +1790,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1807,7 +1804,7 @@
         <v>9</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1821,7 +1818,7 @@
         <v>8</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1835,7 +1832,7 @@
         <v>11</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1849,7 +1846,7 @@
         <v>13</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1863,7 +1860,7 @@
         <v>17</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1877,7 +1874,7 @@
         <v>18</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1891,7 +1888,7 @@
         <v>19</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1905,7 +1902,7 @@
         <v>21</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -1919,7 +1916,7 @@
         <v>23</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -1933,7 +1930,7 @@
         <v>24</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1947,7 +1944,7 @@
         <v>26</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1961,7 +1958,7 @@
         <v>28</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -1975,7 +1972,7 @@
         <v>32</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -1989,7 +1986,7 @@
         <v>33</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -2003,7 +2000,7 @@
         <v>37</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -2017,7 +2014,7 @@
         <v>43</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -2031,7 +2028,7 @@
         <v>38</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -2045,7 +2042,7 @@
         <v>39</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -2059,7 +2056,7 @@
         <v>42</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -2073,40 +2070,40 @@
         <v>44</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="3">
-        <v>22</v>
+      <c r="A23" s="4">
+        <v>23</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="4">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="4">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>49</v>
@@ -2115,12 +2112,12 @@
         <v>55</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="4">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>50</v>
@@ -2129,12 +2126,12 @@
         <v>56</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="4">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>51</v>
@@ -2143,12 +2140,12 @@
         <v>57</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="4">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>52</v>
@@ -2157,12 +2154,12 @@
         <v>58</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="4">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>53</v>
@@ -2171,35 +2168,21 @@
         <v>59</v>
       </c>
       <c r="D29" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="6">
+        <v>30</v>
+      </c>
+      <c r="B30" s="6" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="4">
-        <v>29</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>54</v>
-      </c>
       <c r="C30" s="6" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31" s="6">
-        <v>30</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>